<commit_message>
Matrix info spreadsheet info update
</commit_message>
<xml_diff>
--- a/matrices/matricesInfo.xlsx
+++ b/matrices/matricesInfo.xlsx
@@ -617,7 +617,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,35 +670,35 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>23884</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <f>IF(ISNUMBER(SEARCH("S", A2)),B2*2,B2)</f>
-        <v>23884</v>
+        <v>49</v>
       </c>
       <c r="D2">
-        <v>719290</v>
+        <v>1571</v>
       </c>
       <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2">
+        <v>49</v>
+      </c>
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2">
-        <v>23884</v>
-      </c>
-      <c r="H2">
-        <v>32</v>
-      </c>
       <c r="I2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>4.8153199999999998</v>
+        <v>5.4444400000000002</v>
       </c>
       <c r="K2">
-        <v>13.567500000000001</v>
+        <v>0.24691399999999999</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -706,323 +706,323 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>9027150</v>
+        <v>406858</v>
       </c>
       <c r="C3">
         <f>IF(ISNUMBER(SEARCH("S", A3)),B3*2,B3)</f>
-        <v>18054300</v>
+        <v>813716</v>
       </c>
       <c r="D3">
-        <v>294986795</v>
+        <v>12677170</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="G3">
-        <v>17550675</v>
+        <v>711558</v>
       </c>
       <c r="H3">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>34.845700000000001</v>
+        <v>6.9652700000000003</v>
       </c>
       <c r="K3">
-        <v>1.5789899999999999</v>
+        <v>0.51156800000000002</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>484256</v>
+        <v>4904179</v>
       </c>
       <c r="C4">
         <f>IF(ISNUMBER(SEARCH("S", A4)),B4*2,B4)</f>
-        <v>484256</v>
+        <v>9808358</v>
       </c>
       <c r="D4">
-        <v>10802394</v>
+        <v>163044976</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="G4">
-        <v>484256</v>
+        <v>8580313</v>
       </c>
       <c r="H4">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>20.554200000000002</v>
+        <v>6.9869700000000003</v>
       </c>
       <c r="K4">
-        <v>1.6148100000000001</v>
+        <v>0.65837599999999996</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>1234877</v>
+        <v>328556</v>
       </c>
       <c r="C5">
         <f>IF(ISNUMBER(SEARCH("S", A5)),B5*2,B5)</f>
-        <v>1234877</v>
+        <v>657112</v>
       </c>
       <c r="D5">
-        <v>16012615</v>
+        <v>10113669</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="G5">
-        <v>1234877</v>
+        <v>574458</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>4.1711270000000003</v>
+        <v>6.9501499999999998</v>
       </c>
       <c r="K5">
-        <v>0.90542500000000004</v>
+        <v>0.76873000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>219812</v>
+        <v>1234877</v>
       </c>
       <c r="C6">
         <f>IF(ISNUMBER(SEARCH("S", A6)),B6*2,B6)</f>
-        <v>439624</v>
+        <v>1234877</v>
       </c>
       <c r="D6">
-        <v>5610999</v>
+        <v>16012615</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6">
-        <v>428650</v>
+        <v>1234877</v>
       </c>
       <c r="H6">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>39.060499999999998</v>
+        <v>4.1711270000000003</v>
       </c>
       <c r="K6">
-        <v>237.578</v>
+        <v>0.90542500000000004</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>49</v>
+        <v>1541898</v>
       </c>
       <c r="C7">
         <f>IF(ISNUMBER(SEARCH("S", A7)),B7*2,B7)</f>
-        <v>49</v>
+        <v>3083796</v>
       </c>
       <c r="D7">
-        <v>1571</v>
+        <v>21511862</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="G7">
-        <v>49</v>
+        <v>3083796</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>5.4444400000000002</v>
+        <v>2.8267799999999998</v>
       </c>
       <c r="K7">
-        <v>0.24691399999999999</v>
+        <v>1.05223</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>2034917</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>9027150</v>
+      </c>
+      <c r="C8" s="1">
         <f>IF(ISNUMBER(SEARCH("S", A8)),B8*2,B8)</f>
-        <v>4069834</v>
-      </c>
-      <c r="D8">
-        <v>59698523</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8">
-        <v>4007383</v>
-      </c>
-      <c r="H8">
-        <v>78</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>64.168400000000005</v>
-      </c>
-      <c r="K8">
-        <v>197.578</v>
+        <v>18054300</v>
+      </c>
+      <c r="D8" s="1">
+        <v>294986795</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="1">
+        <v>17550675</v>
+      </c>
+      <c r="H8" s="1">
+        <v>35</v>
+      </c>
+      <c r="I8" s="1">
+        <v>15</v>
+      </c>
+      <c r="J8" s="1">
+        <v>34.845700000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.5789899999999999</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>76367</v>
-      </c>
-      <c r="C9">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>484256</v>
+      </c>
+      <c r="C9" s="1">
         <f>IF(ISNUMBER(SEARCH("S", A9)),B9*2,B9)</f>
-        <v>76367</v>
-      </c>
-      <c r="D9">
-        <v>2303785</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9">
-        <v>76367</v>
-      </c>
-      <c r="H9">
-        <v>62</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9">
-        <v>29.405899999999999</v>
-      </c>
-      <c r="K9">
-        <v>223.41800000000001</v>
+        <v>484256</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10802394</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1">
+        <v>484256</v>
+      </c>
+      <c r="H9" s="1">
+        <v>21</v>
+      </c>
+      <c r="I9" s="1">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1">
+        <v>20.554200000000002</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.6148100000000001</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>1362087</v>
+        <v>492564</v>
       </c>
       <c r="C10">
         <f>IF(ISNUMBER(SEARCH("S", A10)),B10*2,B10)</f>
-        <v>2724174</v>
+        <v>492564</v>
       </c>
       <c r="D10">
-        <v>27894342</v>
+        <v>15636867</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G10">
-        <v>2624331</v>
+        <v>492564</v>
       </c>
       <c r="H10">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10">
-        <v>21.654299999999999</v>
+        <v>4.4999500000000001</v>
       </c>
       <c r="K10">
-        <v>190.238</v>
+        <v>3.7600899999999999</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>64685452</v>
+        <v>3996</v>
       </c>
       <c r="C11">
         <f>IF(ISNUMBER(SEARCH("S", A11)),B11*2,B11)</f>
-        <v>129370904</v>
+        <v>3996</v>
       </c>
       <c r="D11">
-        <v>1741959598</v>
+        <v>124041</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G11">
-        <v>127206144</v>
+        <v>3996</v>
       </c>
       <c r="H11">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="I11">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="J11">
-        <v>58.7622</v>
+        <v>3.996</v>
       </c>
       <c r="K11">
-        <v>19.9954</v>
+        <v>3.9919799999999999</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1030,179 +1030,179 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>766396</v>
+        <v>7353</v>
       </c>
       <c r="C12">
         <f>IF(ISNUMBER(SEARCH("S", A12)),B12*2,B12)</f>
-        <v>766396</v>
+        <v>7353</v>
       </c>
       <c r="D12">
-        <v>15909280</v>
+        <v>219771</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G12">
-        <v>766396</v>
+        <v>7353</v>
       </c>
       <c r="H12">
-        <v>114190</v>
+        <v>12</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12">
-        <v>6.5596399999999999</v>
+        <v>3.6383000000000001</v>
       </c>
       <c r="K12">
-        <v>130681</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>430740</v>
-      </c>
-      <c r="C13">
+        <v>5.7093499999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>27689972</v>
+      </c>
+      <c r="C13" s="1">
         <f>IF(ISNUMBER(SEARCH("S", A13)),B13*2,B13)</f>
-        <v>430740</v>
-      </c>
-      <c r="D13">
-        <v>13509711</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13">
-        <v>430740</v>
-      </c>
-      <c r="H13">
-        <v>27</v>
-      </c>
-      <c r="I13">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>24.090599999999998</v>
-      </c>
-      <c r="K13">
-        <v>18.5656</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27689972</v>
+      </c>
+      <c r="D13" s="1">
+        <v>807404608</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1">
+        <v>27689972</v>
+      </c>
+      <c r="H13" s="1">
+        <v>74</v>
+      </c>
+      <c r="I13" s="1">
+        <v>26</v>
+      </c>
+      <c r="J13" s="1">
+        <v>73.447800000000001</v>
+      </c>
+      <c r="K13" s="1">
+        <v>12.424300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14">
-        <v>492564</v>
+        <v>23884</v>
       </c>
       <c r="C14">
         <f>IF(ISNUMBER(SEARCH("S", A14)),B14*2,B14)</f>
-        <v>492564</v>
+        <v>23884</v>
       </c>
       <c r="D14">
-        <v>15636867</v>
+        <v>719290</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
+        <v>6</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="G14">
-        <v>492564</v>
+        <v>23884</v>
       </c>
       <c r="H14">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="I14">
         <v>2</v>
       </c>
       <c r="J14">
-        <v>4.4999500000000001</v>
+        <v>4.8153199999999998</v>
       </c>
       <c r="K14">
-        <v>3.7600899999999999</v>
+        <v>13.567500000000001</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>1273389</v>
-      </c>
-      <c r="C15">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14883536</v>
+      </c>
+      <c r="C15" s="1">
         <f>IF(ISNUMBER(SEARCH("S", A15)),B15*2,B15)</f>
-        <v>1273389</v>
-      </c>
-      <c r="D15">
-        <v>32904083</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15">
-        <v>1273389</v>
-      </c>
-      <c r="H15">
-        <v>44</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>6.1665299999999998</v>
-      </c>
-      <c r="K15">
-        <v>19.6769</v>
+        <v>29767072</v>
+      </c>
+      <c r="D15" s="1">
+        <v>263408170</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="1">
+        <v>28704672</v>
+      </c>
+      <c r="H15" s="1">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1">
+        <v>5</v>
+      </c>
+      <c r="J15" s="1">
+        <v>27.018699999999999</v>
+      </c>
+      <c r="K15" s="1">
+        <v>13.9511</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>24382</v>
-      </c>
-      <c r="C16">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>430740</v>
+      </c>
+      <c r="C16" s="1">
         <f>IF(ISNUMBER(SEARCH("S", A16)),B16*2,B16)</f>
-        <v>24382</v>
-      </c>
-      <c r="D16">
-        <v>703247</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16">
-        <v>24382</v>
-      </c>
-      <c r="H16">
-        <v>81</v>
-      </c>
-      <c r="I16">
+        <v>430740</v>
+      </c>
+      <c r="D16" s="1">
+        <v>13509711</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J16">
-        <v>31.8719</v>
-      </c>
-      <c r="K16">
-        <v>285.99099999999999</v>
+      <c r="F16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="1">
+        <v>430740</v>
+      </c>
+      <c r="H16" s="1">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1">
+        <v>24.090599999999998</v>
+      </c>
+      <c r="K16" s="1">
+        <v>18.5656</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1210,71 +1210,71 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>8562</v>
+        <v>1273389</v>
       </c>
       <c r="C17">
         <f>IF(ISNUMBER(SEARCH("S", A17)),B17*2,B17)</f>
-        <v>8562</v>
+        <v>1273389</v>
       </c>
       <c r="D17">
-        <v>187366</v>
+        <v>32904083</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G17">
-        <v>8562</v>
+        <v>1273389</v>
       </c>
       <c r="H17">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17">
-        <v>20.581700000000001</v>
+        <v>6.1665299999999998</v>
       </c>
       <c r="K17">
-        <v>39.969299999999997</v>
+        <v>19.6769</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B18">
-        <v>102252</v>
+        <v>64685452</v>
       </c>
       <c r="C18">
         <f>IF(ISNUMBER(SEARCH("S", A18)),B18*2,B18)</f>
-        <v>102252</v>
+        <v>129370904</v>
       </c>
       <c r="D18">
-        <v>2722334</v>
+        <v>1741959598</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G18">
-        <v>102252</v>
+        <v>127206144</v>
       </c>
       <c r="H18">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="J18">
-        <v>21.302499999999998</v>
+        <v>58.7622</v>
       </c>
       <c r="K18">
-        <v>33.634300000000003</v>
+        <v>19.9954</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1282,71 +1282,71 @@
         <v>0</v>
       </c>
       <c r="B19">
-        <v>27689972</v>
+        <v>102252</v>
       </c>
       <c r="C19">
         <f>IF(ISNUMBER(SEARCH("S", A19)),B19*2,B19)</f>
-        <v>27689972</v>
+        <v>102252</v>
       </c>
       <c r="D19">
-        <v>807404608</v>
+        <v>2722334</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19">
-        <v>27689972</v>
+        <v>102252</v>
       </c>
       <c r="H19">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="I19">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>73.447800000000001</v>
+        <v>21.302499999999998</v>
       </c>
       <c r="K19">
-        <v>12.424300000000001</v>
+        <v>33.634300000000003</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B20">
-        <v>14883536</v>
+        <v>8562</v>
       </c>
       <c r="C20">
         <f>IF(ISNUMBER(SEARCH("S", A20)),B20*2,B20)</f>
-        <v>29767072</v>
+        <v>8562</v>
       </c>
       <c r="D20">
-        <v>263408170</v>
+        <v>187366</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G20">
-        <v>28704672</v>
+        <v>8562</v>
       </c>
       <c r="H20">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>27.018699999999999</v>
+        <v>20.581700000000001</v>
       </c>
       <c r="K20">
-        <v>13.9511</v>
+        <v>39.969299999999997</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1390,107 +1390,107 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>3996</v>
+        <v>56934</v>
       </c>
       <c r="C22">
         <f>IF(ISNUMBER(SEARCH("S", A22)),B22*2,B22)</f>
-        <v>3996</v>
+        <v>56934</v>
       </c>
       <c r="D22">
-        <v>124041</v>
+        <v>1501008</v>
       </c>
       <c r="E22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="G22">
-        <v>3996</v>
+        <v>56934</v>
       </c>
       <c r="H22">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22">
-        <v>3.996</v>
+        <v>17.8</v>
       </c>
       <c r="K22">
-        <v>3.9919799999999999</v>
+        <v>189.232</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B23">
-        <v>8185136</v>
+        <v>1362087</v>
       </c>
       <c r="C23">
         <f>IF(ISNUMBER(SEARCH("S", A23)),B23*2,B23)</f>
-        <v>8185136</v>
+        <v>2724174</v>
       </c>
       <c r="D23">
-        <v>265075192</v>
+        <v>27894342</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G23">
-        <v>8185136</v>
+        <v>2624331</v>
       </c>
       <c r="H23">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>50.817300000000003</v>
+        <v>21.654299999999999</v>
       </c>
       <c r="K23">
-        <v>388.02199999999999</v>
+        <v>190.238</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B24">
-        <v>294276</v>
+        <v>2034917</v>
       </c>
       <c r="C24">
         <f>IF(ISNUMBER(SEARCH("S", A24)),B24*2,B24)</f>
-        <v>294276</v>
+        <v>4069834</v>
       </c>
       <c r="D24">
-        <v>7711742</v>
+        <v>59698523</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G24">
-        <v>294276</v>
+        <v>4007383</v>
       </c>
       <c r="H24">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="I24">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>90.769900000000007</v>
+        <v>64.168400000000005</v>
       </c>
       <c r="K24">
-        <v>449.125</v>
+        <v>197.578</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1498,182 +1498,182 @@
         <v>0</v>
       </c>
       <c r="B25">
-        <v>56934</v>
+        <v>76367</v>
       </c>
       <c r="C25">
         <f>IF(ISNUMBER(SEARCH("S", A25)),B25*2,B25)</f>
-        <v>56934</v>
+        <v>76367</v>
       </c>
       <c r="D25">
-        <v>1501008</v>
+        <v>2303785</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="G25">
-        <v>56934</v>
+        <v>76367</v>
       </c>
       <c r="H25">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J25">
-        <v>17.8</v>
+        <v>29.405899999999999</v>
       </c>
       <c r="K25">
-        <v>189.232</v>
+        <v>223.41800000000001</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B26">
-        <v>1541898</v>
+        <v>219812</v>
       </c>
       <c r="C26">
         <f>IF(ISNUMBER(SEARCH("S", A26)),B26*2,B26)</f>
-        <v>3083796</v>
+        <v>439624</v>
       </c>
       <c r="D26">
-        <v>21511862</v>
+        <v>5610999</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="G26">
-        <v>3083796</v>
+        <v>428650</v>
       </c>
       <c r="H26">
-        <v>9</v>
+        <v>150</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>2.8267799999999998</v>
+        <v>39.060499999999998</v>
       </c>
       <c r="K26">
-        <v>1.05223</v>
+        <v>237.578</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B27">
-        <v>328556</v>
+        <v>24382</v>
       </c>
       <c r="C27">
         <f>IF(ISNUMBER(SEARCH("S", A27)),B27*2,B27)</f>
-        <v>657112</v>
+        <v>24382</v>
       </c>
       <c r="D27">
-        <v>10113669</v>
+        <v>703247</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G27">
-        <v>574458</v>
+        <v>24382</v>
       </c>
       <c r="H27">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="J27">
-        <v>6.9501499999999998</v>
+        <v>31.8719</v>
       </c>
       <c r="K27">
-        <v>0.76873000000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>285.99099999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B28">
-        <v>4904179</v>
+        <v>8185136</v>
       </c>
       <c r="C28">
         <f>IF(ISNUMBER(SEARCH("S", A28)),B28*2,B28)</f>
-        <v>9808358</v>
+        <v>8185136</v>
       </c>
       <c r="D28">
-        <v>163044976</v>
+        <v>265075192</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G28">
-        <v>8580313</v>
+        <v>8185136</v>
       </c>
       <c r="H28">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="I28">
         <v>1</v>
       </c>
       <c r="J28">
-        <v>6.9869700000000003</v>
+        <v>50.817300000000003</v>
       </c>
       <c r="K28">
-        <v>0.65837599999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>388.02199999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B29">
-        <v>406858</v>
+        <v>294276</v>
       </c>
       <c r="C29">
         <f>IF(ISNUMBER(SEARCH("S", A29)),B29*2,B29)</f>
-        <v>813716</v>
+        <v>294276</v>
       </c>
       <c r="D29">
-        <v>12677170</v>
+        <v>7711742</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G29">
-        <v>711558</v>
+        <v>294276</v>
       </c>
       <c r="H29">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="I29">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="J29">
-        <v>6.9652700000000003</v>
+        <v>90.769900000000007</v>
       </c>
       <c r="K29">
-        <v>0.51156800000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>449.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1714,41 +1714,41 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>7353</v>
+        <v>766396</v>
       </c>
       <c r="C31">
         <f>IF(ISNUMBER(SEARCH("S", A31)),B31*2,B31)</f>
-        <v>7353</v>
+        <v>766396</v>
       </c>
       <c r="D31">
-        <v>219771</v>
+        <v>15909280</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G31">
-        <v>7353</v>
+        <v>766396</v>
       </c>
       <c r="H31">
-        <v>12</v>
+        <v>114190</v>
       </c>
       <c r="I31">
         <v>1</v>
       </c>
       <c r="J31">
-        <v>3.6383000000000001</v>
+        <v>6.5596399999999999</v>
       </c>
       <c r="K31">
-        <v>5.7093499999999997</v>
+        <v>130681</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K31">
     <sortState ref="A2:K31">
-      <sortCondition ref="E1:E31"/>
+      <sortCondition ref="K1:K31"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>